<commit_message>
add search product test
</commit_message>
<xml_diff>
--- a/ManualTest/Test.xlsx
+++ b/ManualTest/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snc\Desktop\CicekSepetiUITests\ManualTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE3D543-FA76-4109-805F-B4D6F110698B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F04E4-0F4A-446B-9D08-089C08742E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Test ID</t>
   </si>
@@ -137,6 +137,9 @@
 2. E posta ve şifre gir. 
 3. Giriş Yap butonuna tıkla
 4. Hesabım elementini gözlemle.</t>
+  </si>
+  <si>
+    <t>Kullanıcı anasayfa'da olmalı</t>
   </si>
 </sst>
 </file>
@@ -511,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,7 +611,7 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>

</xml_diff>